<commit_message>
added KiCad files for front array
</commit_message>
<xml_diff>
--- a/hardware/reflectance_sensor_array/reflectance_sensor_array-BOM.xlsx
+++ b/hardware/reflectance_sensor_array/reflectance_sensor_array-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shuri\Dropbox\Robotics\github\yozh\hardware\reflectance_sensor_array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8A3ED4-C224-4C39-8B55-D13F83EEB353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834A62CC-2DDF-48F6-9AB2-976EEB265072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67485" yWindow="1710" windowWidth="13890" windowHeight="9045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generic BOM" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
   <si>
     <t>Component</t>
   </si>
@@ -1029,19 +1029,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="23.20703125" customWidth="1"/>
-    <col min="3" max="3" width="23.05078125" customWidth="1"/>
-    <col min="5" max="5" width="8.83984375" style="4"/>
-    <col min="11" max="11" width="16.89453125" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" customWidth="1"/>
+    <col min="3" max="3" width="23.08984375" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" style="4"/>
+    <col min="11" max="11" width="16.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
     </row>
   </sheetData>
@@ -1308,18 +1308,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.83984375" style="4"/>
+    <col min="1" max="1" width="16.08984375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.36328125" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -1333,7 +1335,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1347,84 +1349,73 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="4">
-        <v>15</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>